<commit_message>
setting up framework for writing json and generating graphs
</commit_message>
<xml_diff>
--- a/ScoutingComplex2015/DataEntry/sample_files/template.xlsx
+++ b/ScoutingComplex2015/DataEntry/sample_files/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aravindkoneru/Desktop/Scouting System/ScoutingComplex2015/DataEntry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aravindkoneru/Desktop/Scouting System/ScoutingComplex2015/DataEntry/sample_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>